<commit_message>
multi browser implementation for chrome and firefox and accounting cash
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Makerepayment1.xlsx
@@ -119,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -140,6 +140,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -180,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -209,12 +214,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -230,6 +229,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -619,7 +639,7 @@
         <v>833.33</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>655.89</v>
       </c>
@@ -639,7 +659,7 @@
         <v>84.38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -659,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -679,36 +699,24 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="13"/>
+    </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-    </row>
-    <row r="8" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-    </row>
-    <row r="11" spans="1:10" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="8"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D13" s="13"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="13"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D8" s="12"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -718,10 +726,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -730,104 +738,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="11">
         <v>42005</v>
       </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="9">
         <v>10000</v>
       </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
+      <c r="H2" s="3"/>
       <c r="I2" s="3">
         <v>0</v>
       </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
+      <c r="J2" s="3"/>
       <c r="K2" s="3">
         <v>0</v>
       </c>
       <c r="L2" s="3">
         <v>0</v>
       </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2" s="3">
-        <v>0</v>
-      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="P2" s="3"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
@@ -842,9 +827,7 @@
       <c r="D3" s="11">
         <v>42036</v>
       </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
+      <c r="E3" s="19"/>
       <c r="F3" s="3">
         <v>833.33</v>
       </c>
@@ -870,9 +853,6 @@
         <v>0</v>
       </c>
       <c r="N3" s="3">
-        <v>0</v>
-      </c>
-      <c r="O3" s="3">
         <v>0</v>
       </c>
       <c r="P3" s="3">
@@ -889,12 +869,8 @@
       <c r="C4" s="11">
         <v>42064</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="3">
         <v>833.33</v>
       </c>
@@ -920,9 +896,6 @@
         <v>0</v>
       </c>
       <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3">
         <v>0</v>
       </c>
       <c r="P4" s="3">
@@ -939,12 +912,8 @@
       <c r="C5" s="11">
         <v>42095</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0</v>
-      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="3">
         <v>833.33</v>
       </c>
@@ -970,9 +939,6 @@
         <v>0</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
         <v>0</v>
       </c>
       <c r="P5" s="3">
@@ -989,12 +955,8 @@
       <c r="C6" s="11">
         <v>42125</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="3">
         <v>833.33</v>
       </c>
@@ -1020,9 +982,6 @@
         <v>0</v>
       </c>
       <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="O6" s="3">
         <v>0</v>
       </c>
       <c r="P6" s="3">
@@ -1039,12 +998,8 @@
       <c r="C7" s="11">
         <v>42156</v>
       </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="3">
         <v>833.33</v>
       </c>
@@ -1070,9 +1025,6 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>0</v>
-      </c>
-      <c r="O7" s="3">
         <v>0</v>
       </c>
       <c r="P7" s="3">
@@ -1089,12 +1041,8 @@
       <c r="C8" s="11">
         <v>42186</v>
       </c>
-      <c r="D8" s="3">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="3">
         <v>833.33</v>
       </c>
@@ -1120,9 +1068,6 @@
         <v>0</v>
       </c>
       <c r="N8" s="3">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3">
         <v>0</v>
       </c>
       <c r="P8" s="3">
@@ -1139,12 +1084,8 @@
       <c r="C9" s="11">
         <v>42217</v>
       </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="3">
         <v>833.33</v>
       </c>
@@ -1170,9 +1111,6 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>0</v>
-      </c>
-      <c r="O9" s="3">
         <v>0</v>
       </c>
       <c r="P9" s="3">
@@ -1189,12 +1127,8 @@
       <c r="C10" s="11">
         <v>42248</v>
       </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0</v>
-      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="3">
         <v>833.33</v>
       </c>
@@ -1220,9 +1154,6 @@
         <v>0</v>
       </c>
       <c r="N10" s="3">
-        <v>0</v>
-      </c>
-      <c r="O10" s="3">
         <v>0</v>
       </c>
       <c r="P10" s="3">
@@ -1239,12 +1170,8 @@
       <c r="C11" s="11">
         <v>42278</v>
       </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="3">
         <v>833.33</v>
       </c>
@@ -1270,9 +1197,6 @@
         <v>0</v>
       </c>
       <c r="N11" s="3">
-        <v>0</v>
-      </c>
-      <c r="O11" s="3">
         <v>0</v>
       </c>
       <c r="P11" s="3">
@@ -1289,12 +1213,8 @@
       <c r="C12" s="11">
         <v>42309</v>
       </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>0</v>
-      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="3">
         <v>833.33</v>
       </c>
@@ -1320,9 +1240,6 @@
         <v>0</v>
       </c>
       <c r="N12" s="3">
-        <v>0</v>
-      </c>
-      <c r="O12" s="3">
         <v>0</v>
       </c>
       <c r="P12" s="3">
@@ -1339,12 +1256,8 @@
       <c r="C13" s="11">
         <v>42339</v>
       </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="3">
         <v>833.33</v>
       </c>
@@ -1370,9 +1283,6 @@
         <v>0</v>
       </c>
       <c r="N13" s="3">
-        <v>0</v>
-      </c>
-      <c r="O13" s="3">
         <v>0</v>
       </c>
       <c r="P13" s="3">
@@ -1389,12 +1299,8 @@
       <c r="C14" s="11">
         <v>42370</v>
       </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="3">
         <v>833.37</v>
       </c>
@@ -1422,18 +1328,9 @@
       <c r="N14" s="3">
         <v>0</v>
       </c>
-      <c r="O14" s="3">
-        <v>0</v>
-      </c>
       <c r="P14" s="3">
         <v>841.86</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1442,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1457,11 +1354,11 @@
     <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -1489,86 +1386,75 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>2622</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
+        <v>19</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="21">
         <v>42036</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="20">
         <v>935.25</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="20">
         <v>833.33</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="20">
         <v>101.92</v>
       </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0</v>
-      </c>
-      <c r="J2" s="7">
+      <c r="H2" s="20">
+        <v>0</v>
+      </c>
+      <c r="I2" s="20">
+        <v>0</v>
+      </c>
+      <c r="J2" s="22">
         <v>9166.67</v>
       </c>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>2621</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="20">
+        <v>17</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="21">
         <v>42005</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="25">
         <v>10000</v>
       </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="9">
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20">
+        <v>0</v>
+      </c>
+      <c r="I3" s="20">
+        <v>0</v>
+      </c>
+      <c r="J3" s="25">
         <v>10000</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="3"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Loan RBI, Variable Instalments
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/101-RBI-EPP-DB-DL-REC-NOCOM-RNI-CTPD-SAR-MD-TR-1-ONTIME-Makerepayment1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mifosx-e2e-testing\Mifos Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="9" r:id="rId1"/>
@@ -118,7 +123,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -260,6 +265,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -307,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,9 +348,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,6 +400,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -726,10 +768,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -737,7 +779,7 @@
     <col min="3" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>12</v>
       </c>
@@ -777,17 +819,18 @@
       <c r="M1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="16"/>
+      <c r="O1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="11">
@@ -812,9 +855,10 @@
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O2" s="3"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -852,14 +896,15 @@
       <c r="M3" s="3">
         <v>0</v>
       </c>
-      <c r="N3" s="3">
-        <v>0</v>
-      </c>
-      <c r="P3" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N3" s="3"/>
+      <c r="O3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -895,14 +940,15 @@
       <c r="M4" s="3">
         <v>0</v>
       </c>
-      <c r="N4" s="3">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3">
+      <c r="N4" s="3"/>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3">
         <v>917.71</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -938,14 +984,15 @@
       <c r="M5" s="3">
         <v>0</v>
       </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
+      <c r="N5" s="3"/>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
         <v>926.75</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -981,14 +1028,15 @@
       <c r="M6" s="3">
         <v>0</v>
       </c>
-      <c r="N6" s="3">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
+      <c r="N6" s="3"/>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
         <v>907.3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1024,14 +1072,15 @@
       <c r="M7" s="3">
         <v>0</v>
       </c>
-      <c r="N7" s="3">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3">
+      <c r="N7" s="3"/>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
         <v>901.28</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1067,14 +1116,15 @@
       <c r="M8" s="3">
         <v>0</v>
       </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3">
+      <c r="N8" s="3"/>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
         <v>890.86</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1110,14 +1160,15 @@
       <c r="M9" s="3">
         <v>0</v>
       </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3">
+      <c r="N9" s="3"/>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
         <v>884.29</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1153,14 +1204,15 @@
       <c r="M10" s="3">
         <v>0</v>
       </c>
-      <c r="N10" s="3">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3">
+      <c r="N10" s="3"/>
+      <c r="O10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
         <v>875.8</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1196,14 +1248,15 @@
       <c r="M11" s="3">
         <v>0</v>
       </c>
-      <c r="N11" s="3">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3">
+      <c r="N11" s="3"/>
+      <c r="O11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
         <v>866.21</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1239,14 +1292,15 @@
       <c r="M12" s="3">
         <v>0</v>
       </c>
-      <c r="N12" s="3">
-        <v>0</v>
-      </c>
-      <c r="P12" s="3">
+      <c r="N12" s="3"/>
+      <c r="O12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
         <v>858.81</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1282,14 +1336,15 @@
       <c r="M13" s="3">
         <v>0</v>
       </c>
-      <c r="N13" s="3">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3">
+      <c r="N13" s="3"/>
+      <c r="O13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
         <v>849.77</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1325,10 +1380,11 @@
       <c r="M14" s="3">
         <v>0</v>
       </c>
-      <c r="N14" s="3">
-        <v>0</v>
-      </c>
-      <c r="P14" s="3">
+      <c r="N14" s="3"/>
+      <c r="O14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
         <v>841.86</v>
       </c>
     </row>
@@ -1341,7 +1397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>